<commit_message>
deleted Tonner 2017 scripts
</commit_message>
<xml_diff>
--- a/data/CLS/Day.275_YPD/20180928_16.biological.stats_0.corrected.xlsx
+++ b/data/CLS/Day.275_YPD/20180928_16.biological.stats_0.corrected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\Box Sync\JTL_Lab\Lab.Notebook\20170903_DR_Evolution\data\CLS\Day.275_YPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73CFF56-CAD3-422F-AC89-8B94347F8862}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672446A7-750F-42A6-A5CA-1D05F9B4F2D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-14400" yWindow="4185" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20180422_16.biological.lx" sheetId="1" r:id="rId1"/>
@@ -2071,7 +2071,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>